<commit_message>
Got most of the code ported over to ARM but it needs lots of work still
</commit_message>
<xml_diff>
--- a/files/Pin chart LED.xlsx
+++ b/files/Pin chart LED.xlsx
@@ -98,18 +98,6 @@
     <t>black stripe</t>
   </si>
   <si>
-    <t>a0</t>
-  </si>
-  <si>
-    <t>a1</t>
-  </si>
-  <si>
-    <t>a2</t>
-  </si>
-  <si>
-    <t>a3</t>
-  </si>
-  <si>
     <t>d2</t>
   </si>
   <si>
@@ -153,6 +141,18 @@
   </si>
   <si>
     <t>row selector - 3to8 decoder to select one of 8 logical rows (2 physical rows at a time)</t>
+  </si>
+  <si>
+    <t>d10</t>
+  </si>
+  <si>
+    <t>d11</t>
+  </si>
+  <si>
+    <t>d12</t>
+  </si>
+  <si>
+    <t>d13</t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,16 +564,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -584,7 +584,7 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -595,7 +595,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -606,7 +606,7 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -617,7 +617,7 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -628,7 +628,7 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -639,7 +639,7 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -650,7 +650,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -661,10 +661,10 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -675,10 +675,10 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -689,10 +689,10 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -703,10 +703,10 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -717,7 +717,7 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>